<commit_message>
Modified 06/08/2024 01:48:53 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (UC) - Color-wise Data & Graphs/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (UC) - Color-wise Data & Graphs/2020_cars_combined.xlsx
@@ -735,25 +735,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11.68831168831169</v>
+        <v>11.69</v>
       </c>
       <c r="C2" t="n">
-        <v>34.41558441558442</v>
+        <v>34.42</v>
       </c>
       <c r="D2" t="n">
-        <v>27.27272727272727</v>
+        <v>27.27</v>
       </c>
       <c r="E2" t="n">
-        <v>9.740259740259742</v>
+        <v>9.74</v>
       </c>
       <c r="F2" t="n">
-        <v>2.597402597402597</v>
+        <v>2.6</v>
       </c>
       <c r="G2" t="n">
-        <v>7.792207792207792</v>
+        <v>7.79</v>
       </c>
       <c r="H2" t="n">
-        <v>6.493506493506493</v>
+        <v>6.49</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -772,19 +772,19 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>46.98795180722892</v>
+        <v>46.99</v>
       </c>
       <c r="D3" t="n">
-        <v>36.74698795180723</v>
+        <v>36.75</v>
       </c>
       <c r="E3" t="n">
-        <v>5.421686746987952</v>
+        <v>5.42</v>
       </c>
       <c r="F3" t="n">
-        <v>7.228915662650602</v>
+        <v>7.23</v>
       </c>
       <c r="G3" t="n">
-        <v>3.614457831325301</v>
+        <v>3.61</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -803,25 +803,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17.30769230769231</v>
+        <v>17.31</v>
       </c>
       <c r="C4" t="n">
-        <v>23.07692307692308</v>
+        <v>23.08</v>
       </c>
       <c r="D4" t="n">
-        <v>25.64102564102564</v>
+        <v>25.64</v>
       </c>
       <c r="E4" t="n">
-        <v>12.17948717948718</v>
+        <v>12.18</v>
       </c>
       <c r="F4" t="n">
-        <v>5.769230769230769</v>
+        <v>5.77</v>
       </c>
       <c r="G4" t="n">
-        <v>8.333333333333332</v>
+        <v>8.33</v>
       </c>
       <c r="H4" t="n">
-        <v>7.692307692307693</v>
+        <v>7.69</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -840,19 +840,19 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>49.68152866242038</v>
+        <v>49.68</v>
       </c>
       <c r="D5" t="n">
-        <v>17.19745222929936</v>
+        <v>17.2</v>
       </c>
       <c r="E5" t="n">
-        <v>22.29299363057325</v>
+        <v>22.29</v>
       </c>
       <c r="F5" t="n">
-        <v>6.369426751592357</v>
+        <v>6.37</v>
       </c>
       <c r="G5" t="n">
-        <v>4.45859872611465</v>
+        <v>4.46</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -874,22 +874,22 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>29.51807228915663</v>
+        <v>29.52</v>
       </c>
       <c r="D6" t="n">
-        <v>24.69879518072289</v>
+        <v>24.7</v>
       </c>
       <c r="E6" t="n">
-        <v>19.27710843373494</v>
+        <v>19.28</v>
       </c>
       <c r="F6" t="n">
-        <v>9.036144578313253</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="G6" t="n">
-        <v>13.85542168674699</v>
+        <v>13.86</v>
       </c>
       <c r="H6" t="n">
-        <v>3.614457831325301</v>
+        <v>3.61</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -908,22 +908,22 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>22.52747252747253</v>
+        <v>22.53</v>
       </c>
       <c r="D7" t="n">
-        <v>36.26373626373626</v>
+        <v>36.26</v>
       </c>
       <c r="E7" t="n">
-        <v>16.48351648351648</v>
+        <v>16.48</v>
       </c>
       <c r="F7" t="n">
-        <v>9.890109890109891</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="G7" t="n">
-        <v>12.63736263736264</v>
+        <v>12.64</v>
       </c>
       <c r="H7" t="n">
-        <v>2.197802197802198</v>
+        <v>2.2</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -939,25 +939,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>15.13157894736842</v>
+        <v>15.13</v>
       </c>
       <c r="C8" t="n">
-        <v>36.84210526315789</v>
+        <v>36.84</v>
       </c>
       <c r="D8" t="n">
-        <v>19.73684210526316</v>
+        <v>19.74</v>
       </c>
       <c r="E8" t="n">
-        <v>9.868421052631579</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="F8" t="n">
-        <v>3.947368421052631</v>
+        <v>3.95</v>
       </c>
       <c r="G8" t="n">
-        <v>9.210526315789473</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="H8" t="n">
-        <v>5.263157894736842</v>
+        <v>5.26</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -973,25 +973,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>20.98765432098765</v>
+        <v>20.99</v>
       </c>
       <c r="C9" t="n">
-        <v>8.024691358024691</v>
+        <v>8.02</v>
       </c>
       <c r="D9" t="n">
-        <v>20.37037037037037</v>
+        <v>20.37</v>
       </c>
       <c r="E9" t="n">
-        <v>22.22222222222222</v>
+        <v>22.22</v>
       </c>
       <c r="F9" t="n">
-        <v>8.641975308641975</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="G9" t="n">
-        <v>12.34567901234568</v>
+        <v>12.35</v>
       </c>
       <c r="H9" t="n">
-        <v>7.407407407407407</v>
+        <v>7.41</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -1010,19 +1010,19 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>14.19753086419753</v>
+        <v>14.2</v>
       </c>
       <c r="D10" t="n">
-        <v>51.85185185185185</v>
+        <v>51.85</v>
       </c>
       <c r="E10" t="n">
-        <v>22.83950617283951</v>
+        <v>22.84</v>
       </c>
       <c r="F10" t="n">
-        <v>8.641975308641975</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="G10" t="n">
-        <v>2.469135802469136</v>
+        <v>2.47</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1031,7 +1031,7 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>99.99999999999999</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
@@ -1041,25 +1041,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.80722891566265</v>
+        <v>1.81</v>
       </c>
       <c r="C11" t="n">
-        <v>22.28915662650602</v>
+        <v>22.29</v>
       </c>
       <c r="D11" t="n">
-        <v>25.30120481927711</v>
+        <v>25.3</v>
       </c>
       <c r="E11" t="n">
-        <v>21.68674698795181</v>
+        <v>21.69</v>
       </c>
       <c r="F11" t="n">
-        <v>12.65060240963855</v>
+        <v>12.65</v>
       </c>
       <c r="G11" t="n">
-        <v>12.65060240963855</v>
+        <v>12.65</v>
       </c>
       <c r="H11" t="n">
-        <v>3.614457831325301</v>
+        <v>3.61</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Modified 06/08/2024 02:27:48 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (UC) - Color-wise Data & Graphs/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (UC) - Color-wise Data & Graphs/2020_cars_combined.xlsx
@@ -735,25 +735,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11.69</v>
+        <v>11.68831168831169</v>
       </c>
       <c r="C2" t="n">
-        <v>34.42</v>
+        <v>34.41558441558442</v>
       </c>
       <c r="D2" t="n">
-        <v>27.27</v>
+        <v>27.27272727272727</v>
       </c>
       <c r="E2" t="n">
-        <v>9.74</v>
+        <v>9.740259740259742</v>
       </c>
       <c r="F2" t="n">
-        <v>2.6</v>
+        <v>2.597402597402597</v>
       </c>
       <c r="G2" t="n">
-        <v>7.79</v>
+        <v>7.792207792207792</v>
       </c>
       <c r="H2" t="n">
-        <v>6.49</v>
+        <v>6.493506493506493</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -772,19 +772,19 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>46.99</v>
+        <v>46.98795180722892</v>
       </c>
       <c r="D3" t="n">
-        <v>36.75</v>
+        <v>36.74698795180723</v>
       </c>
       <c r="E3" t="n">
-        <v>5.42</v>
+        <v>5.421686746987952</v>
       </c>
       <c r="F3" t="n">
-        <v>7.23</v>
+        <v>7.228915662650602</v>
       </c>
       <c r="G3" t="n">
-        <v>3.61</v>
+        <v>3.614457831325301</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -803,25 +803,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17.31</v>
+        <v>17.30769230769231</v>
       </c>
       <c r="C4" t="n">
-        <v>23.08</v>
+        <v>23.07692307692308</v>
       </c>
       <c r="D4" t="n">
-        <v>25.64</v>
+        <v>25.64102564102564</v>
       </c>
       <c r="E4" t="n">
-        <v>12.18</v>
+        <v>12.17948717948718</v>
       </c>
       <c r="F4" t="n">
-        <v>5.77</v>
+        <v>5.769230769230769</v>
       </c>
       <c r="G4" t="n">
-        <v>8.33</v>
+        <v>8.333333333333332</v>
       </c>
       <c r="H4" t="n">
-        <v>7.69</v>
+        <v>7.692307692307693</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -840,19 +840,19 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>49.68</v>
+        <v>49.68152866242038</v>
       </c>
       <c r="D5" t="n">
-        <v>17.2</v>
+        <v>17.19745222929936</v>
       </c>
       <c r="E5" t="n">
-        <v>22.29</v>
+        <v>22.29299363057325</v>
       </c>
       <c r="F5" t="n">
-        <v>6.37</v>
+        <v>6.369426751592357</v>
       </c>
       <c r="G5" t="n">
-        <v>4.46</v>
+        <v>4.45859872611465</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -874,22 +874,22 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>29.52</v>
+        <v>29.51807228915663</v>
       </c>
       <c r="D6" t="n">
-        <v>24.7</v>
+        <v>24.69879518072289</v>
       </c>
       <c r="E6" t="n">
-        <v>19.28</v>
+        <v>19.27710843373494</v>
       </c>
       <c r="F6" t="n">
-        <v>9.039999999999999</v>
+        <v>9.036144578313253</v>
       </c>
       <c r="G6" t="n">
-        <v>13.86</v>
+        <v>13.85542168674699</v>
       </c>
       <c r="H6" t="n">
-        <v>3.61</v>
+        <v>3.614457831325301</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -908,22 +908,22 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>22.53</v>
+        <v>22.52747252747253</v>
       </c>
       <c r="D7" t="n">
-        <v>36.26</v>
+        <v>36.26373626373626</v>
       </c>
       <c r="E7" t="n">
-        <v>16.48</v>
+        <v>16.48351648351648</v>
       </c>
       <c r="F7" t="n">
-        <v>9.890000000000001</v>
+        <v>9.890109890109891</v>
       </c>
       <c r="G7" t="n">
-        <v>12.64</v>
+        <v>12.63736263736264</v>
       </c>
       <c r="H7" t="n">
-        <v>2.2</v>
+        <v>2.197802197802198</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -939,25 +939,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>15.13</v>
+        <v>15.13157894736842</v>
       </c>
       <c r="C8" t="n">
-        <v>36.84</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="D8" t="n">
-        <v>19.74</v>
+        <v>19.73684210526316</v>
       </c>
       <c r="E8" t="n">
-        <v>9.869999999999999</v>
+        <v>9.868421052631579</v>
       </c>
       <c r="F8" t="n">
-        <v>3.95</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="G8" t="n">
-        <v>9.210000000000001</v>
+        <v>9.210526315789473</v>
       </c>
       <c r="H8" t="n">
-        <v>5.26</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -973,25 +973,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>20.99</v>
+        <v>20.98765432098765</v>
       </c>
       <c r="C9" t="n">
-        <v>8.02</v>
+        <v>8.024691358024691</v>
       </c>
       <c r="D9" t="n">
-        <v>20.37</v>
+        <v>20.37037037037037</v>
       </c>
       <c r="E9" t="n">
-        <v>22.22</v>
+        <v>22.22222222222222</v>
       </c>
       <c r="F9" t="n">
-        <v>8.640000000000001</v>
+        <v>8.641975308641975</v>
       </c>
       <c r="G9" t="n">
-        <v>12.35</v>
+        <v>12.34567901234568</v>
       </c>
       <c r="H9" t="n">
-        <v>7.41</v>
+        <v>7.407407407407407</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -1010,19 +1010,19 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>14.2</v>
+        <v>14.19753086419753</v>
       </c>
       <c r="D10" t="n">
-        <v>51.85</v>
+        <v>51.85185185185185</v>
       </c>
       <c r="E10" t="n">
-        <v>22.84</v>
+        <v>22.83950617283951</v>
       </c>
       <c r="F10" t="n">
-        <v>8.640000000000001</v>
+        <v>8.641975308641975</v>
       </c>
       <c r="G10" t="n">
-        <v>2.47</v>
+        <v>2.469135802469136</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1031,7 +1031,7 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>100</v>
+        <v>99.99999999999999</v>
       </c>
     </row>
     <row r="11">
@@ -1041,25 +1041,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.81</v>
+        <v>1.80722891566265</v>
       </c>
       <c r="C11" t="n">
-        <v>22.29</v>
+        <v>22.28915662650602</v>
       </c>
       <c r="D11" t="n">
-        <v>25.3</v>
+        <v>25.30120481927711</v>
       </c>
       <c r="E11" t="n">
-        <v>21.69</v>
+        <v>21.68674698795181</v>
       </c>
       <c r="F11" t="n">
-        <v>12.65</v>
+        <v>12.65060240963855</v>
       </c>
       <c r="G11" t="n">
-        <v>12.65</v>
+        <v>12.65060240963855</v>
       </c>
       <c r="H11" t="n">
-        <v>3.61</v>
+        <v>3.614457831325301</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Modified 06/08/2024 04:47:21 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (UC) - Color-wise Data & Graphs/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (UC) - Color-wise Data & Graphs/2020_cars_combined.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Graphs" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -137,236 +136,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>10</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>26</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>10</col>
-      <colOff>0</colOff>
-      <row>26</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>52</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>10</col>
-      <colOff>0</colOff>
-      <row>52</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="6" name="Image 6" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>78</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="7" name="Image 7" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>10</col>
-      <colOff>0</colOff>
-      <row>78</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="8" name="Image 8" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>104</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="9" name="Image 9" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1071,29 +840,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K105"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1"/>
-    <row r="27"/>
-    <row r="53"/>
-    <row r="79"/>
-    <row r="105"/>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified 06/08/2024 04:49:22 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (UC) - Color-wise Data & Graphs/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (UC) - Color-wise Data & Graphs/2020_cars_combined.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Graphs" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -134,6 +135,1550 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Default green</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Default green</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$B$2:$B$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Average: 6.69</v>
+          </tx>
+          <spPr>
+            <a:ln w="30000">
+              <a:solidFill>
+                <a:srgbClr val="FFA500"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$B$2:$B$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>%-age</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Green</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Green</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$C$2:$C$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Average: 28.76</v>
+          </tx>
+          <spPr>
+            <a:ln w="30000">
+              <a:solidFill>
+                <a:srgbClr val="FFA500"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$C$2:$C$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>%-age</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Yellow</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Yellow</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$D$2:$D$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Average: 28.51</v>
+          </tx>
+          <spPr>
+            <a:ln w="30000">
+              <a:solidFill>
+                <a:srgbClr val="FFA500"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$D$2:$D$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>%-age</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Orange</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Orange</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$E$2:$E$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Average: 16.20</v>
+          </tx>
+          <spPr>
+            <a:ln w="30000">
+              <a:solidFill>
+                <a:srgbClr val="FFA500"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$E$2:$E$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>%-age</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Brown</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Brown</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$F$2:$F$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Average: 7.48</v>
+          </tx>
+          <spPr>
+            <a:ln w="30000">
+              <a:solidFill>
+                <a:srgbClr val="FFA500"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$F$2:$F$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>%-age</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Red</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Red</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$G$2:$G$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Average: 8.74</v>
+          </tx>
+          <spPr>
+            <a:ln w="30000">
+              <a:solidFill>
+                <a:srgbClr val="FFA500"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$G$2:$G$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>%-age</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Default Red</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Default Red</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$H$2:$H$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Average: 3.63</v>
+          </tx>
+          <spPr>
+            <a:ln w="30000">
+              <a:solidFill>
+                <a:srgbClr val="FFA500"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$H$2:$H$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>%-age</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Blue</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Blue</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$I$2:$I$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Average: 0.00</v>
+          </tx>
+          <spPr>
+            <a:ln w="30000">
+              <a:solidFill>
+                <a:srgbClr val="FFA500"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$I$2:$I$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>%-age</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Predicted headform score (excluding blue points)</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Predicted headform score (excluding blue points)</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$J$2:$J$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Average: 100.00</v>
+          </tx>
+          <spPr>
+            <a:ln w="30000">
+              <a:solidFill>
+                <a:srgbClr val="FFA500"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Graphs'!$A$2:$A$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Graphs'!$J$2:$J$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>%-age</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>30</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>45</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="4" name="Chart 4"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>60</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="5" name="Chart 5"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>75</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="6" name="Chart 6"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>90</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="7" name="Chart 7"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>105</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="8" name="Chart 8"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>120</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="9" name="Chart 9"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -840,4 +2385,23 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>